<commit_message>
Update dinosaurs const; Update new map info"
</commit_message>
<xml_diff>
--- a/const/dinosaurs.xlsx
+++ b/const/dinosaurs.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="0" windowWidth="30340" windowHeight="18180"/>
+    <workbookView xWindow="-480" yWindow="180" windowWidth="21720" windowHeight="13620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="dinosaurs_avai" sheetId="6" r:id="rId1"/>
     <sheet name="experience" sheetId="4" r:id="rId2"/>
     <sheet name="skill_avai" sheetId="7" r:id="rId3"/>
     <sheet name="dinosaurs_old" sheetId="3" r:id="rId4"/>
+    <sheet name="calc" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="145">
   <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -505,6 +507,102 @@
   </si>
   <si>
     <t>自叠加</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>毒牙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使敌中毒</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>断筋</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>敌方敏捷-</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>尖刺</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>反伤</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>咆哮</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>使敌方受到伤害提高</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>撕裂</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,4,5,8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>霸王龙</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,3,4,6,8,9,10,11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,4,6,8,9,10,11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,3,4,5,7,10,11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,6,8,9,10,11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,3,4,8,9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,4,6,7,9,10,11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,3,5,7,8,9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2,3,4,5,7,8,9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>防</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -515,7 +613,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,6 +717,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -784,7 +890,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -835,10 +941,17 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="23" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="标题" xfId="23" builtinId="15"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -861,29 +974,28 @@
     <cellStyle name="超链接" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="45" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1182,18 +1294,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:X25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="18" max="18" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.875" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="15.75" customWidth="1"/>
+    <col min="17" max="17" width="20.5" customWidth="1"/>
+    <col min="18" max="18" width="23" customWidth="1"/>
+    <col min="22" max="22" width="14.625" customWidth="1"/>
+    <col min="23" max="23" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1260,8 +1379,11 @@
       <c r="V1" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" s="5" customFormat="1">
+      <c r="W1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1275,10 +1397,10 @@
         <v>114</v>
       </c>
       <c r="E2" s="3">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F2" s="3">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G2" s="3">
         <v>6</v>
@@ -1286,17 +1408,17 @@
       <c r="H2" s="3">
         <v>20</v>
       </c>
-      <c r="I2" s="3">
-        <v>6</v>
-      </c>
-      <c r="J2" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K2" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="L2" s="3">
-        <v>3</v>
+      <c r="I2" s="2">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="K2" s="2">
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="L2" s="2">
+        <v>12</v>
       </c>
       <c r="M2" s="14">
         <v>1</v>
@@ -1328,8 +1450,14 @@
       <c r="V2" s="3">
         <v>3600</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" s="5" customFormat="1">
+      <c r="W2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1343,10 +1471,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="3">
-        <v>125</v>
+        <v>400</v>
       </c>
       <c r="F3" s="3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G3" s="3">
         <v>8</v>
@@ -1354,17 +1482,17 @@
       <c r="H3" s="3">
         <v>18</v>
       </c>
-      <c r="I3" s="3">
-        <v>8</v>
-      </c>
-      <c r="J3" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="K3" s="3">
-        <v>1.8</v>
-      </c>
-      <c r="L3" s="3">
-        <v>2.4</v>
+      <c r="I3" s="2">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2">
+        <v>10.4</v>
+      </c>
+      <c r="K3" s="2">
+        <v>7.2</v>
+      </c>
+      <c r="L3" s="2">
+        <v>9.6</v>
       </c>
       <c r="M3" s="14">
         <v>1</v>
@@ -1396,8 +1524,14 @@
       <c r="V3" s="3">
         <v>7200</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" s="5" customFormat="1">
+      <c r="W3" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1411,10 +1545,10 @@
         <v>115</v>
       </c>
       <c r="E4" s="3">
-        <v>125</v>
+        <v>400</v>
       </c>
       <c r="F4" s="3">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G4" s="3">
         <v>10</v>
@@ -1422,17 +1556,17 @@
       <c r="H4" s="3">
         <v>14</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
+        <v>36</v>
+      </c>
+      <c r="J4" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="K4" s="2">
         <v>8</v>
       </c>
-      <c r="J4" s="3">
-        <v>1.6</v>
-      </c>
-      <c r="K4" s="3">
-        <v>2</v>
-      </c>
-      <c r="L4" s="3">
-        <v>1.4</v>
+      <c r="L4" s="2">
+        <v>5.6000000000000005</v>
       </c>
       <c r="M4" s="14">
         <v>1</v>
@@ -1464,8 +1598,14 @@
       <c r="V4" s="3">
         <v>7200</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" s="5" customFormat="1">
+      <c r="W4" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1479,10 +1619,10 @@
         <v>22</v>
       </c>
       <c r="E5" s="3">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="F5" s="3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G5" s="3">
         <v>16</v>
@@ -1490,17 +1630,17 @@
       <c r="H5" s="3">
         <v>12</v>
       </c>
-      <c r="I5" s="3">
-        <v>6</v>
-      </c>
-      <c r="J5" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="K5" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="L5" s="3">
-        <v>2.2000000000000002</v>
+      <c r="I5" s="2">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2">
+        <v>9.6</v>
+      </c>
+      <c r="K5" s="2">
+        <v>10.4</v>
+      </c>
+      <c r="L5" s="2">
+        <v>8.7999999999999989</v>
       </c>
       <c r="M5" s="14">
         <v>1</v>
@@ -1532,8 +1672,14 @@
       <c r="V5" s="3">
         <v>3600</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" s="5" customFormat="1">
+      <c r="W5" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1547,10 +1693,10 @@
         <v>30</v>
       </c>
       <c r="E6" s="3">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="F6" s="3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G6" s="3">
         <v>18</v>
@@ -1558,17 +1704,17 @@
       <c r="H6" s="3">
         <v>18</v>
       </c>
-      <c r="I6" s="3">
-        <v>6</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1.4</v>
-      </c>
-      <c r="K6" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="L6" s="3">
-        <v>2.8</v>
+      <c r="I6" s="2">
+        <v>28</v>
+      </c>
+      <c r="J6" s="2">
+        <v>8</v>
+      </c>
+      <c r="K6" s="2">
+        <v>11.200000000000001</v>
+      </c>
+      <c r="L6" s="2">
+        <v>11.200000000000001</v>
       </c>
       <c r="M6" s="14">
         <v>1</v>
@@ -1600,8 +1746,14 @@
       <c r="V6" s="3">
         <v>3600</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" s="5" customFormat="1">
+      <c r="W6" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1615,10 +1767,10 @@
         <v>34</v>
       </c>
       <c r="E7" s="3">
-        <v>125</v>
+        <v>400</v>
       </c>
       <c r="F7" s="3">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G7" s="3">
         <v>10</v>
@@ -1626,17 +1778,17 @@
       <c r="H7" s="3">
         <v>20</v>
       </c>
-      <c r="I7" s="3">
-        <v>6</v>
-      </c>
-      <c r="J7" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="K7" s="3">
-        <v>2</v>
-      </c>
-      <c r="L7" s="3">
-        <v>3</v>
+      <c r="I7" s="2">
+        <v>30</v>
+      </c>
+      <c r="J7" s="2">
+        <v>10.8</v>
+      </c>
+      <c r="K7" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="L7" s="2">
+        <v>12</v>
       </c>
       <c r="M7" s="14">
         <v>1</v>
@@ -1668,8 +1820,14 @@
       <c r="V7" s="3">
         <v>3600</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" s="5" customFormat="1">
+      <c r="W7" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1683,28 +1841,28 @@
         <v>19</v>
       </c>
       <c r="E8" s="3">
-        <v>150</v>
+        <v>400</v>
       </c>
       <c r="F8" s="3">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G8" s="3">
         <v>18</v>
       </c>
       <c r="H8" s="3">
-        <v>12</v>
-      </c>
-      <c r="I8" s="3">
-        <v>6</v>
-      </c>
-      <c r="J8" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="K8" s="3">
-        <v>2.8</v>
-      </c>
-      <c r="L8" s="3">
-        <v>2.2000000000000002</v>
+        <v>18</v>
+      </c>
+      <c r="I8" s="2">
+        <v>28</v>
+      </c>
+      <c r="J8" s="2">
+        <v>11.200000000000001</v>
+      </c>
+      <c r="K8" s="2">
+        <v>11.200000000000001</v>
+      </c>
+      <c r="L8" s="2">
+        <v>11.2</v>
       </c>
       <c r="M8" s="14">
         <v>1</v>
@@ -1736,8 +1894,14 @@
       <c r="V8" s="3">
         <v>7200</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" s="5" customFormat="1">
+      <c r="W8" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1751,28 +1915,28 @@
         <v>48</v>
       </c>
       <c r="E9" s="3">
-        <v>300</v>
+        <v>700</v>
       </c>
       <c r="F9" s="3">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G9" s="3">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H9" s="3">
         <v>4</v>
       </c>
-      <c r="I9" s="3">
-        <v>10</v>
-      </c>
-      <c r="J9" s="3">
-        <v>2.4</v>
-      </c>
-      <c r="K9" s="3">
-        <v>3</v>
-      </c>
-      <c r="L9" s="3">
-        <v>1.4</v>
+      <c r="I9" s="2">
+        <v>44</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9.6</v>
+      </c>
+      <c r="K9" s="2">
+        <v>12</v>
+      </c>
+      <c r="L9" s="2">
+        <v>5.6000000000000005</v>
       </c>
       <c r="M9" s="14">
         <v>1</v>
@@ -1804,8 +1968,14 @@
       <c r="V9" s="3">
         <v>10800</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" s="5" customFormat="1">
+      <c r="W9" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1819,10 +1989,10 @@
         <v>51</v>
       </c>
       <c r="E10" s="3">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="F10" s="3">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="G10" s="3">
         <v>12</v>
@@ -1830,17 +2000,17 @@
       <c r="H10" s="3">
         <v>14</v>
       </c>
-      <c r="I10" s="3">
-        <v>8</v>
-      </c>
-      <c r="J10" s="3">
-        <v>3</v>
-      </c>
-      <c r="K10" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="L10" s="3">
-        <v>2.4</v>
+      <c r="I10" s="2">
+        <v>36</v>
+      </c>
+      <c r="J10" s="2">
+        <v>12</v>
+      </c>
+      <c r="K10" s="2">
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="L10" s="2">
+        <v>8.8000000000000007</v>
       </c>
       <c r="M10" s="14">
         <v>1</v>
@@ -1872,33 +2042,79 @@
       <c r="V10" s="3">
         <v>7200</v>
       </c>
-    </row>
-    <row r="15" spans="1:22">
+      <c r="W10" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="X10" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
       <c r="S15" s="5"/>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
       <c r="S16" s="5"/>
     </row>
-    <row r="17" spans="19:19">
+    <row r="17" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
       <c r="S17" s="5"/>
     </row>
-    <row r="18" spans="19:19">
+    <row r="18" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
       <c r="S18" s="5"/>
     </row>
-    <row r="19" spans="19:19">
+    <row r="19" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
       <c r="S19" s="5"/>
     </row>
-    <row r="20" spans="19:19">
+    <row r="20" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
       <c r="S20" s="5"/>
     </row>
-    <row r="21" spans="19:19">
+    <row r="21" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
       <c r="S21" s="5"/>
     </row>
-    <row r="22" spans="19:19">
+    <row r="22" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
       <c r="S22" s="5"/>
     </row>
-    <row r="23" spans="19:19">
+    <row r="23" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
       <c r="S23" s="5"/>
+    </row>
+    <row r="24" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="9:19" x14ac:dyDescent="0.15">
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1914,18 +2130,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="2"/>
+    <col min="1" max="2" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -1933,7 +2149,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1941,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1950,7 +2166,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1959,7 +2175,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1968,7 +2184,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1977,7 +2193,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1986,7 +2202,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1995,7 +2211,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2004,7 +2220,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2013,7 +2229,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2022,7 +2238,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2031,7 +2247,7 @@
         <v>1310</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2040,7 +2256,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2049,7 +2265,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2058,7 +2274,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2067,7 +2283,7 @@
         <v>2390</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2076,7 +2292,7 @@
         <v>2710</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2085,7 +2301,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2094,7 +2310,7 @@
         <v>3410</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2103,7 +2319,7 @@
         <v>3790</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2112,7 +2328,7 @@
         <v>4190</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2121,7 +2337,7 @@
         <v>4610</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2130,7 +2346,7 @@
         <v>5050</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2139,7 +2355,7 @@
         <v>5510</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2148,7 +2364,7 @@
         <v>5990</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2157,7 +2373,7 @@
         <v>6490</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2166,7 +2382,7 @@
         <v>7010</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2175,7 +2391,7 @@
         <v>7550</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2184,7 +2400,7 @@
         <v>8110</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2193,7 +2409,7 @@
         <v>8690</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2202,7 +2418,7 @@
         <v>9290</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2211,7 +2427,7 @@
         <v>9910</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2220,7 +2436,7 @@
         <v>10550</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2229,7 +2445,7 @@
         <v>11210</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2238,7 +2454,7 @@
         <v>11890</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2247,7 +2463,7 @@
         <v>12590</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2256,7 +2472,7 @@
         <v>13310</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2265,7 +2481,7 @@
         <v>14050</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2274,7 +2490,7 @@
         <v>14810</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2283,7 +2499,7 @@
         <v>15590</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2292,7 +2508,7 @@
         <v>16390</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2301,7 +2517,7 @@
         <v>17210</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2310,7 +2526,7 @@
         <v>18050</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2319,7 +2535,7 @@
         <v>18910</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2328,7 +2544,7 @@
         <v>19790</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2337,7 +2553,7 @@
         <v>20690</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2346,7 +2562,7 @@
         <v>21610</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2355,7 +2571,7 @@
         <v>22550</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2364,7 +2580,7 @@
         <v>23510</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2373,7 +2589,7 @@
         <v>24490</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2382,7 +2598,7 @@
         <v>25490</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2391,10 +2607,271 @@
         <v>26510</v>
       </c>
     </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2">
+        <f t="shared" ref="B53:B79" si="2">10*(A52+1)*(A52+1)+10*(A52+1)-10</f>
+        <v>27550</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2">
+        <f t="shared" si="2"/>
+        <v>28610</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2">
+        <f t="shared" si="2"/>
+        <v>29690</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2">
+        <f t="shared" si="2"/>
+        <v>30790</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2">
+        <f t="shared" si="2"/>
+        <v>31910</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2">
+        <f t="shared" si="2"/>
+        <v>33050</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2">
+        <f t="shared" si="2"/>
+        <v>34210</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2">
+        <f t="shared" si="2"/>
+        <v>35390</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2">
+        <f t="shared" si="2"/>
+        <v>36590</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2">
+        <f t="shared" si="2"/>
+        <v>37810</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2">
+        <f t="shared" si="2"/>
+        <v>39050</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2">
+        <f t="shared" si="2"/>
+        <v>40310</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2">
+        <f t="shared" si="2"/>
+        <v>41590</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="B66" s="2">
+        <f t="shared" si="2"/>
+        <v>42890</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2">
+        <f t="shared" si="2"/>
+        <v>44210</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2">
+        <f t="shared" si="2"/>
+        <v>45550</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2">
+        <f t="shared" si="2"/>
+        <v>46910</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+      <c r="B70" s="2">
+        <f t="shared" si="2"/>
+        <v>48290</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="B71" s="2">
+        <f t="shared" si="2"/>
+        <v>49690</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2">
+        <f t="shared" si="2"/>
+        <v>51110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+      <c r="B73" s="2">
+        <f t="shared" si="2"/>
+        <v>52550</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="B74" s="2">
+        <f t="shared" si="2"/>
+        <v>54010</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" s="2">
+        <f t="shared" si="2"/>
+        <v>55490</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="B76" s="2">
+        <f t="shared" si="2"/>
+        <v>56990</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="B77" s="2">
+        <f t="shared" si="2"/>
+        <v>58510</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+      <c r="B78" s="2">
+        <f t="shared" si="2"/>
+        <v>60050</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+      <c r="B79" s="2">
+        <f t="shared" si="2"/>
+        <v>61610</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="B80" s="2">
+        <f t="shared" ref="B80:B81" si="3">10*(A79+1)*(A79+1)+10*(A79+1)-10</f>
+        <v>63190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+      <c r="B81" s="2">
+        <f t="shared" si="3"/>
+        <v>64790</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2405,25 +2882,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="2"/>
-    <col min="5" max="5" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="43.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="12.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="2"/>
+    <col min="5" max="5" width="13.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="43.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="22" thickBot="1">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2461,7 +2938,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" thickTop="1">
+    <row r="2" spans="1:12" ht="14.25" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2490,7 +2967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2519,7 +2996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2548,7 +3025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2580,7 +3057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2609,7 +3086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2638,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2667,7 +3144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2696,7 +3173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2725,7 +3202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2754,7 +3231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2781,6 +3258,124 @@
       </c>
       <c r="K12" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="2">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" s="2">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="2">
+        <v>14</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D16" s="2">
+        <v>15</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2799,24 +3394,24 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:Q1"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>94</v>
       </c>
@@ -2884,7 +3479,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="5" customFormat="1">
+    <row r="2" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -2952,7 +3547,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="5" customFormat="1">
+    <row r="3" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3020,7 +3615,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -3088,7 +3683,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="5" customFormat="1">
+    <row r="5" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3156,7 +3751,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="5" customFormat="1">
+    <row r="6" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3224,7 +3819,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -3292,7 +3887,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="5" customFormat="1">
+    <row r="8" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3360,7 +3955,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="5" customFormat="1">
+    <row r="9" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3428,7 +4023,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -3496,7 +4091,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -3564,7 +4159,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="5" customFormat="1">
+    <row r="12" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3632,7 +4227,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -3700,7 +4295,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -3768,7 +4363,7 @@
         <v>7200</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="5" customFormat="1">
+    <row r="15" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3836,7 +4431,7 @@
         <v>10800</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="5" customFormat="1">
+    <row r="16" spans="1:22" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3914,4 +4509,494 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1">
+        <f>dinosaurs_avai!E2+dinosaurs_avai!I2*50</f>
+        <v>1300</v>
+      </c>
+      <c r="D1">
+        <f>dinosaurs_avai!F2+dinosaurs_avai!J2*80</f>
+        <v>592</v>
+      </c>
+      <c r="E1">
+        <f>dinosaurs_avai!G2+dinosaurs_avai!K2*80</f>
+        <v>518</v>
+      </c>
+      <c r="F1">
+        <f>dinosaurs_avai!H2+dinosaurs_avai!L2*80</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <f>dinosaurs_avai!E3+dinosaurs_avai!I3*50</f>
+        <v>1800</v>
+      </c>
+      <c r="D2">
+        <f>dinosaurs_avai!F3+dinosaurs_avai!J3*80</f>
+        <v>850</v>
+      </c>
+      <c r="E2">
+        <f>dinosaurs_avai!G3+dinosaurs_avai!K3*80</f>
+        <v>584</v>
+      </c>
+      <c r="F2">
+        <f>dinosaurs_avai!H3+dinosaurs_avai!L3*80</f>
+        <v>786</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <f>dinosaurs_avai!E4+dinosaurs_avai!I4*50</f>
+        <v>2200</v>
+      </c>
+      <c r="D3">
+        <f>dinosaurs_avai!F4+dinosaurs_avai!J4*80</f>
+        <v>698</v>
+      </c>
+      <c r="E3">
+        <f>dinosaurs_avai!G4+dinosaurs_avai!K4*80</f>
+        <v>650</v>
+      </c>
+      <c r="F3">
+        <f>dinosaurs_avai!H4+dinosaurs_avai!L4*80</f>
+        <v>462.00000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4">
+        <f>dinosaurs_avai!E5+dinosaurs_avai!I5*50</f>
+        <v>2000</v>
+      </c>
+      <c r="D4">
+        <f>dinosaurs_avai!F5+dinosaurs_avai!J5*80</f>
+        <v>786</v>
+      </c>
+      <c r="E4">
+        <f>dinosaurs_avai!G5+dinosaurs_avai!K5*80</f>
+        <v>848</v>
+      </c>
+      <c r="F4">
+        <f>dinosaurs_avai!H5+dinosaurs_avai!L5*80</f>
+        <v>715.99999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5">
+        <f>dinosaurs_avai!E6+dinosaurs_avai!I6*50</f>
+        <v>1800</v>
+      </c>
+      <c r="D5">
+        <f>dinosaurs_avai!F6+dinosaurs_avai!J6*80</f>
+        <v>658</v>
+      </c>
+      <c r="E5">
+        <f>dinosaurs_avai!G6+dinosaurs_avai!K6*80</f>
+        <v>914.00000000000011</v>
+      </c>
+      <c r="F5">
+        <f>dinosaurs_avai!H6+dinosaurs_avai!L6*80</f>
+        <v>914.00000000000011</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <f>dinosaurs_avai!E7+dinosaurs_avai!I7*50</f>
+        <v>1900</v>
+      </c>
+      <c r="D6">
+        <f>dinosaurs_avai!F7+dinosaurs_avai!J7*80</f>
+        <v>888</v>
+      </c>
+      <c r="E6">
+        <f>dinosaurs_avai!G7+dinosaurs_avai!K7*80</f>
+        <v>618</v>
+      </c>
+      <c r="F6">
+        <f>dinosaurs_avai!H7+dinosaurs_avai!L7*80</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7">
+        <f>dinosaurs_avai!E8+dinosaurs_avai!I8*50</f>
+        <v>1800</v>
+      </c>
+      <c r="D7">
+        <f>dinosaurs_avai!F8+dinosaurs_avai!J8*80</f>
+        <v>920.00000000000011</v>
+      </c>
+      <c r="E7">
+        <f>dinosaurs_avai!G8+dinosaurs_avai!K8*80</f>
+        <v>914.00000000000011</v>
+      </c>
+      <c r="F7">
+        <f>dinosaurs_avai!H8+dinosaurs_avai!L8*80</f>
+        <v>914</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8">
+        <f>dinosaurs_avai!E9+dinosaurs_avai!I9*50</f>
+        <v>2900</v>
+      </c>
+      <c r="D8">
+        <f>dinosaurs_avai!F9+dinosaurs_avai!J9*80</f>
+        <v>786</v>
+      </c>
+      <c r="E8">
+        <f>dinosaurs_avai!G9+dinosaurs_avai!K9*80</f>
+        <v>988</v>
+      </c>
+      <c r="F8">
+        <f>dinosaurs_avai!H9+dinosaurs_avai!L9*80</f>
+        <v>452.00000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <f>dinosaurs_avai!E10+dinosaurs_avai!I10*50</f>
+        <v>2300</v>
+      </c>
+      <c r="D9">
+        <f>dinosaurs_avai!F10+dinosaurs_avai!J10*80</f>
+        <v>1000</v>
+      </c>
+      <c r="E9">
+        <f>dinosaurs_avai!G10+dinosaurs_avai!K10*80</f>
+        <v>715.99999999999989</v>
+      </c>
+      <c r="F9">
+        <f>dinosaurs_avai!H10+dinosaurs_avai!L10*80</f>
+        <v>718</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="H11" t="s">
+        <v>143</v>
+      </c>
+      <c r="I11" t="s">
+        <v>144</v>
+      </c>
+      <c r="J11" t="s">
+        <v>141</v>
+      </c>
+      <c r="K11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="G12">
+        <v>136</v>
+      </c>
+      <c r="H12">
+        <v>40</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12:J29" si="0">H12*5*(1/(1+I12/G12))</f>
+        <v>191.54929577464787</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>1000</v>
+      </c>
+      <c r="I13">
+        <v>1000</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>454.54545454545456</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="G14">
+        <v>136</v>
+      </c>
+      <c r="H14">
+        <v>1000</v>
+      </c>
+      <c r="I14">
+        <v>988</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>604.98220640569389</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="G15">
+        <v>100</v>
+      </c>
+      <c r="H15">
+        <v>1000</v>
+      </c>
+      <c r="I15">
+        <v>518</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>809.06148867313925</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.15">
+      <c r="G16">
+        <v>136</v>
+      </c>
+      <c r="H16">
+        <v>40</v>
+      </c>
+      <c r="I16">
+        <v>988</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>24.199288256227756</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G17">
+        <v>136</v>
+      </c>
+      <c r="H17">
+        <v>40</v>
+      </c>
+      <c r="I17">
+        <v>518</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>41.590214067278289</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G18">
+        <v>136</v>
+      </c>
+      <c r="H18">
+        <v>40</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>191.54929577464787</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G19">
+        <v>136</v>
+      </c>
+      <c r="H19">
+        <v>40</v>
+      </c>
+      <c r="I19">
+        <v>28</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>165.85365853658539</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>1000</v>
+      </c>
+      <c r="I20">
+        <v>650</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>666.66666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>26</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>122.64150943396226</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G22">
+        <v>100</v>
+      </c>
+      <c r="H22">
+        <v>26</v>
+      </c>
+      <c r="I22">
+        <v>28</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>101.5625</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>18</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>84.905660377358487</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="H24">
+        <v>18</v>
+      </c>
+      <c r="I24">
+        <v>28</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>70.3125</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G25">
+        <v>100</v>
+      </c>
+      <c r="H25">
+        <v>40</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>188.67924528301884</v>
+      </c>
+    </row>
+    <row r="26" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G26">
+        <v>136</v>
+      </c>
+      <c r="H26">
+        <v>40</v>
+      </c>
+      <c r="I26">
+        <v>260</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>68.686868686868678</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G27">
+        <v>136</v>
+      </c>
+      <c r="H27">
+        <v>800</v>
+      </c>
+      <c r="I27">
+        <v>1000</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>478.87323943661983</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G28">
+        <v>136</v>
+      </c>
+      <c r="H28">
+        <v>800</v>
+      </c>
+      <c r="I28">
+        <v>600</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>739.13043478260863</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10" x14ac:dyDescent="0.15">
+      <c r="G29">
+        <v>100</v>
+      </c>
+      <c r="H29">
+        <v>800</v>
+      </c>
+      <c r="I29">
+        <v>700</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>